<commit_message>
casino game image test some chenges
</commit_message>
<xml_diff>
--- a/craftBetAutomation/src/test/java/testData/dataOld.xlsx
+++ b/craftBetAutomation/src/test/java/testData/dataOld.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nerses Khachatryan\Desktop\Git_craftBet_TestAutomation\CraftBet_JavaFrameWork\craftBetAutomation\src\test\java\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77900E2-0393-4389-8378-2665C3281F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="2655" windowWidth="21600" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="588" yWindow="564" windowWidth="15996" windowHeight="5244"/>
   </bookViews>
   <sheets>
     <sheet name="brokenIMG" sheetId="1" r:id="rId1"/>
@@ -20,28 +14,97 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>235 ---&gt; https://resources.craftbet.com/products/      this is not valid src response cod is --&gt; 403</t>
-  </si>
-  <si>
-    <t>236 ---&gt; https://resources.craftbet.com/products/evolution/fpdealornodeal.png      this is not valid src response cod is --&gt; 404</t>
-  </si>
-  <si>
-    <t xml:space="preserve">533 ---&gt; https://resources.%7Bp%7D/products/BankoftheNile.jpg      this is not valid src with exception --&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">733 ---&gt; https://resources.%7Bp%7D/products/BookOfSouls.jpg      this is not valid src with exception --&gt; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">890 ---&gt; https://resources.%7Bp%7D/products/CheekyFruits6Deluxe.jpg      this is not valid src with exception --&gt; </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+  <si>
+    <t>179 ---&gt; https://resources.craftbet.com/products/      this is not valid src response cod is --&gt; 403</t>
+  </si>
+  <si>
+    <t>180 ---&gt; https://resources.craftbet.com/products/evolution/fpdealornodeal.png      this is not valid src response cod is --&gt; 404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">477 ---&gt; https://resources.%7Bp%7D/products/BankoftheNile.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">677 ---&gt; https://resources.%7Bp%7D/products/BookOfSouls.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">834 ---&gt; https://resources.%7Bp%7D/products/CheekyFruits6Deluxe.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1145 ---&gt; https://resources.%7Bp%7D/products/Dream3Team.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1201 ---&gt; https://resources.%7Bp%7D/products/EliteofEvil:PortalofGold.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1223 ---&gt; https://resources.%7Bp%7D/products/EternalShogi%C2%B7jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1349 ---&gt; https://resources.%7Bp%7D/products/FootballStarDeluxe.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1411 ---&gt; https://resources.%7Bp%7D/products/FruitPunchUp%C2%B7jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1432 ---&gt; https://resources.%7Bp%7D/products/Fruitsand777's%C2%B7jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1625 ---&gt; https://resources.%7Bp%7D/products/goldilocks.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t>1690 ---&gt; https://static.egamings.com/games/leander/?attrick_?eroes.jpg      this is not valid src response cod is --&gt; 403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1795 ---&gt; https://resources.%7Bp%7D/products/hotink.jpeg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2043 ---&gt; https://resources.%7Bp%7D/products/LaraJonesisCleopatra%C2%B7jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2182 ---&gt; https://resources.%7Bp%7D/products/LuckyRiches:Hyperspins.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2314 ---&gt; https://resources.%7Bp%7D/products/Meganova%C2%B7jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2341 ---&gt; https://resources.%7Bp%7D/products/MidnightMadness.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2589 ---&gt; https://resources.%7Bp%7D/products/Pentagram5000.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2678 ---&gt; https://resources.%7Bp%7D/products/Popstar.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2917 ---&gt; https://resources.%7Bp%7D/products/RomanPower.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2972 ---&gt; https://resources.%7Bp%7D/products/SamanthaFoxt%C2%B7jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t>3229 ---&gt; https://static.egamings.com/games/mg/supeitup.jpeg      this is not valid src response cod is --&gt; 404</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3233 ---&gt; https://resources.%7Bp%7D/products/SuperBarXPullTab.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3265 ---&gt; https://resources.%7Bp%7D/products/SuperSync.jpg      this is not valid src with exception --&gt; </t>
+  </si>
+  <si>
+    <t>3315 ---&gt; https://static.egamings.com/games/mg/Terminator2.jpg      this is not valid src response cod is --&gt; 404</t>
+  </si>
+  <si>
+    <t>3320 ---&gt; https://resources.craftbet.com/products/      this is not valid src response cod is --&gt; 403</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3714 ---&gt; https://resources.%7Bp%7D/products/WildReelse.jpg      this is not valid src with exception --&gt; </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -78,14 +141,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -132,7 +187,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -164,27 +219,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,24 +253,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,39 +428,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="121.5703125" customWidth="1"/>
+    <col min="1" max="1" width="106.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>